<commit_message>
Azure Security Benchmark v3 spreadsheet
</commit_message>
<xml_diff>
--- a/Azure Security Benchmark/3.0/azure-security-benchmark-v3.0.xlsx
+++ b/Azure Security Benchmark/3.0/azure-security-benchmark-v3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/chcheng1_microsoft_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{718726AC-5B3C-41FD-9D6D-1D395CCB2C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{718726AC-5B3C-41FD-9D6D-1D395CCB2C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{946133D8-707A-48CA-9186-912A1DB279A1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{30BFAFB3-652A-4F32-916F-A5B0C74C3635}"/>
   </bookViews>
@@ -682,11 +682,6 @@
 Set the network boundary and service scope where data in transit encryption is mandatory inside and outside of the network. While this is optional for traffic on private networks, this is critical for traffic on external and public networks. </t>
   </si>
   <si>
-    <t>Enforce secure transfer in services such as Azure Storage, where a native data in transit encryption feature is built in. 
-Enforce HTTPS for workload web application and services by ensuring that any clients connecting to your Azure resources use transportation layer security (TLS) v1.2 or later. For remote management of VMs, use SSH (for Linux) or RDP/TLS (for Windows) instead of an unencrypted protocol. 
-Note: Data in transit encryption is enabled for all Azure traffic travelling between Azure datacenters. TLS v1.2 or later is enabled on most Azure PaaS services by default.</t>
-  </si>
-  <si>
     <t>Double encryption for Azure data in transit: 
 https://docs.microsoft.com/azure/security/fundamentals/double-encryption#data-in-transit
 Understand encryption in transit with Azure: 
@@ -3601,12 +3596,17 @@
 https://docs.microsoft.com/azure/cloud-adoption-framework/secure/devsecops-controls 
 </t>
   </si>
+  <si>
+    <t>Enforce secure transfer in services such as Azure Storage, where a native data in transit encryption feature is built in. 
+Enforce HTTPS for workload web application and services by ensuring that any clients connecting to your Azure resources use transportation layer security (TLS) v1.2 or later. For remote management of VMs, use SSH (for Linux) or RDP/TLS (for Windows) instead of an unencrypted protocol. 
+Note: Data in transit encryption is enabled for all Azure traffic traveling between Azure datacenters. TLS v1.2 or later is enabled on most Azure PaaS services by default.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3672,6 +3672,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="22"/>
@@ -4250,31 +4251,31 @@
   <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="9" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:3" ht="32.450000000000003">
+    <row r="1" spans="2:3" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="31"/>
     </row>
-    <row r="3" spans="2:3" ht="140.44999999999999" customHeight="1" thickBot="1">
+    <row r="3" spans="2:3" ht="140.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="33"/>
     </row>
-    <row r="5" spans="2:3" ht="15" thickBot="1"/>
-    <row r="6" spans="2:3">
+    <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
@@ -4282,7 +4283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>4</v>
       </c>
@@ -4290,7 +4291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>6</v>
       </c>
@@ -4298,7 +4299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>8</v>
       </c>
@@ -4306,7 +4307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -4314,7 +4315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>10</v>
       </c>
@@ -4322,7 +4323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>12</v>
       </c>
@@ -4330,7 +4331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>14</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
         <v>16</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>18</v>
       </c>
@@ -4354,7 +4355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="28.9">
+    <row r="16" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
         <v>20</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="43.15">
+    <row r="17" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
         <v>22</v>
       </c>
@@ -4388,20 +4389,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="20" customWidth="1"/>
     <col min="2" max="4" width="17" style="20" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" style="20" customWidth="1"/>
     <col min="6" max="6" width="17" style="20" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="71.42578125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="113.28515625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="106.7109375" customWidth="1"/>
-    <col min="11" max="11" width="72.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="71.44140625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="113.33203125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="106.6640625" customWidth="1"/>
+    <col min="11" max="11" width="72.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="26" customFormat="1">
+    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>4</v>
       </c>
@@ -4438,7 +4439,7 @@
       <c r="L1" s="25"/>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" ht="408.6" customHeight="1">
+    <row r="2" spans="1:13" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -4473,7 +4474,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="174" customHeight="1">
+    <row r="3" spans="1:13" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -4508,7 +4509,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="360">
+    <row r="4" spans="1:13" ht="360" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -4543,7 +4544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="187.15">
+    <row r="5" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="144">
+    <row r="6" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -4613,7 +4614,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="244.9">
+    <row r="7" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -4648,7 +4649,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="158.44999999999999">
+    <row r="8" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>83</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="158.44999999999999">
+    <row r="9" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>90</v>
       </c>
@@ -4718,7 +4719,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="129.6">
+    <row r="10" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>97</v>
       </c>
@@ -4753,7 +4754,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="364.15" customHeight="1">
+    <row r="11" spans="1:13" ht="364.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>105</v>
       </c>
@@ -4788,7 +4789,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="209.45" customHeight="1">
+    <row r="12" spans="1:13" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>113</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="115.15">
+    <row r="13" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>124</v>
       </c>
@@ -4858,7 +4859,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="187.9" customHeight="1">
+    <row r="14" spans="1:13" ht="187.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>133</v>
       </c>
@@ -4884,88 +4885,88 @@
         <v>139</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="K14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="158.44999999999999">
-      <c r="A15" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>114</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="158.44999999999999">
-      <c r="A16" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>114</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="216">
-      <c r="A17" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>114</v>
@@ -4977,30 +4978,30 @@
         <v>98</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F17" s="11">
         <v>3.6</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="I17" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="J17" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="K17" s="5" t="s">
+    </row>
+    <row r="18" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="187.15">
-      <c r="A18" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>114</v>
@@ -5012,30 +5013,30 @@
         <v>98</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F18" s="11">
         <v>3.6</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="I18" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="J18" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="172.9">
-      <c r="A19" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>114</v>
@@ -5047,103 +5048,103 @@
         <v>98</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F19" s="11">
         <v>3.6</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="J19" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="248.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="248.45" customHeight="1">
-      <c r="A20" s="15" t="s">
+      <c r="B20" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="C20" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="J20" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="K20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="259.14999999999998">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="K21" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="158.44999999999999">
-      <c r="A22" s="15" t="s">
-        <v>197</v>
-      </c>
       <c r="B22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>98</v>
@@ -5152,33 +5153,33 @@
         <v>98</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="J22" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="K22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:11" ht="230.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="230.45" customHeight="1">
-      <c r="A23" s="15" t="s">
-        <v>205</v>
-      </c>
       <c r="B23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>98</v>
@@ -5187,243 +5188,243 @@
         <v>98</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>98</v>
       </c>
       <c r="G23" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="J23" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="216.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="216.6" customHeight="1">
-      <c r="A24" s="15" t="s">
+      <c r="B24" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>98</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="J24" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="K24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="201.6">
-      <c r="A25" s="15" t="s">
+      <c r="B25" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="J25" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="244.9">
-      <c r="A26" s="15" t="s">
+      <c r="B26" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="F26" s="7">
         <v>7.2</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="J26" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="K26" s="5" t="s">
+    </row>
+    <row r="27" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="172.9">
-      <c r="A27" s="15" t="s">
+      <c r="B27" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="J27" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="K27" s="5" t="s">
+    </row>
+    <row r="28" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="158.44999999999999">
-      <c r="A28" s="15" t="s">
+      <c r="B28" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>98</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H28" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="I28" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="J28" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K28" s="5" t="s">
+    </row>
+    <row r="29" spans="1:11" ht="288" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="288">
-      <c r="A29" s="15" t="s">
+      <c r="B29" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="C29" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="I29" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="J29" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="K29" s="5" t="s">
+    </row>
+    <row r="30" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="158.44999999999999">
-      <c r="A30" s="15" t="s">
-        <v>268</v>
-      </c>
       <c r="B30" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>98</v>
@@ -5432,103 +5433,103 @@
         <v>98</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="I30" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="J30" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="K30" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="115.15">
-      <c r="A31" s="15" t="s">
+      <c r="B31" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="G31" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="I31" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="J31" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="K31" s="5" t="s">
+    </row>
+    <row r="32" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="201.6">
-      <c r="A32" s="15" t="s">
+      <c r="B32" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="H32" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="J32" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="K32" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="158.44999999999999">
-      <c r="A33" s="15" t="s">
-        <v>292</v>
-      </c>
       <c r="B33" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>98</v>
@@ -5537,1153 +5538,1153 @@
         <v>98</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>98</v>
       </c>
       <c r="G33" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="I33" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="J33" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="K33" s="5" t="s">
+    </row>
+    <row r="34" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="201.6">
-      <c r="A34" s="15" t="s">
+      <c r="B34" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>98</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="J34" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="K34" s="5" t="s">
+    </row>
+    <row r="35" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="158.44999999999999">
-      <c r="A35" s="15" t="s">
+      <c r="B35" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="G35" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="H35" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="K35" s="5" t="s">
+    </row>
+    <row r="36" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="115.15">
-      <c r="A36" s="15" t="s">
+      <c r="B36" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>98</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="J36" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="K36" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="K36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="158.44999999999999">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G37" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="J37" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="K37" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="K37" s="5" t="s">
+    </row>
+    <row r="38" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="216">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="G38" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="158.44999999999999">
-      <c r="A39" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="F39" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="216">
-      <c r="A40" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>344</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F40" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="K40" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="288" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="K40" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="288">
-      <c r="A41" s="1" t="s">
+      <c r="B41" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="J41" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="K41" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="K41" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="230.45">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="J42" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="K42" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="K42" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="216">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="G43" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="J43" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="K43" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="K43" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="201.6">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="G44" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="K44" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="K44" s="5" t="s">
+    </row>
+    <row r="45" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="409.6" customHeight="1">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="H45" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="J45" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="409.6" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="F46" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="F46" s="5" t="s">
+      <c r="G46" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="J46" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="K46" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="360" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="K46" s="5" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="360" customHeight="1">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F47" s="5">
         <v>10.8</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J47" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="K47" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="K47" s="5" t="s">
+    </row>
+    <row r="48" spans="1:11" ht="244.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="244.9" customHeight="1">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="J48" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="K48" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="K48" s="5" t="s">
+    </row>
+    <row r="49" spans="1:11" ht="374.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="374.45" customHeight="1">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="G49" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="J49" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="K49" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="K49" s="5" t="s">
+    </row>
+    <row r="50" spans="1:11" ht="274.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="274.14999999999998" customHeight="1">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="F50" s="5">
         <v>10.4</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="J50" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="J50" s="9" t="s">
+      <c r="K50" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="K50" s="5" t="s">
+    </row>
+    <row r="51" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="11" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="244.9">
-      <c r="A51" s="11" t="s">
+      <c r="B51" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="C51" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>446</v>
       </c>
       <c r="F51" s="5">
         <v>2.4</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="J51" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="J51" s="10" t="s">
+      <c r="K51" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="K51" s="5" t="s">
+    </row>
+    <row r="52" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="11" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="230.45">
-      <c r="A52" s="11" t="s">
+      <c r="B52" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>454</v>
-      </c>
       <c r="E52" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F52" s="5">
         <v>6.3</v>
       </c>
       <c r="G52" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="J52" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="K52" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="K52" s="5" t="s">
+    </row>
+    <row r="53" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="11" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="201.6">
-      <c r="A53" s="11" t="s">
+      <c r="B53" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B53" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="F53" s="5">
         <v>2.4</v>
       </c>
       <c r="G53" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="J53" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="K53" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="K53" s="5" t="s">
+    </row>
+    <row r="54" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A54" s="11" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="72">
-      <c r="A54" s="11" t="s">
+      <c r="B54" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G54" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="J54" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="K54" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="K54" s="5" t="s">
+    </row>
+    <row r="55" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="11" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="230.45">
-      <c r="A55" s="11" t="s">
+      <c r="B55" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>478</v>
       </c>
       <c r="F55" s="5">
         <v>6.3</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="J55" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="J55" s="10" t="s">
+      <c r="K55" s="5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="K55" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="172.9">
-      <c r="A56" s="11" t="s">
+      <c r="B56" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="5" t="s">
         <v>486</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>487</v>
       </c>
       <c r="F56" s="5">
         <v>11.5</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="I56" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="I56" s="2" t="s">
+      <c r="J56" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="J56" s="5" t="s">
+      <c r="K56" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="K56" s="5" t="s">
+    </row>
+    <row r="57" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="11" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="158.44999999999999">
-      <c r="A57" s="11" t="s">
+      <c r="B57" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>495</v>
-      </c>
       <c r="E57" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F57" s="5">
         <v>5.0999999999999996</v>
       </c>
       <c r="G57" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="J57" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="J57" s="5" t="s">
+      <c r="K57" s="5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="K57" s="5" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="158.44999999999999">
-      <c r="A58" s="11" t="s">
+      <c r="B58" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="F58" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="G58" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="J58" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="J58" s="5" t="s">
+      <c r="K58" s="5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="K58" s="5" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="158.44999999999999">
-      <c r="A59" s="11" t="s">
+      <c r="B59" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="18" t="s">
         <v>512</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>513</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="J59" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="J59" s="10" t="s">
+      <c r="K59" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="K59" s="5" t="s">
+    </row>
+    <row r="60" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="11" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="259.14999999999998">
-      <c r="A60" s="11" t="s">
+      <c r="B60" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="18" t="s">
         <v>521</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>522</v>
       </c>
       <c r="F60" s="2">
         <v>3.4</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="I60" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="J60" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="K60" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="K60" s="5" t="s">
+    </row>
+    <row r="61" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="129.6">
-      <c r="A61" s="11" t="s">
+      <c r="B61" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E61" s="18" t="s">
         <v>528</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>529</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="J61" s="10" t="s">
         <v>532</v>
       </c>
-      <c r="J61" s="10" t="s">
+      <c r="K61" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="K61" s="5" t="s">
+    </row>
+    <row r="62" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="11" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="115.15">
-      <c r="A62" s="11" t="s">
+      <c r="B62" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="18" t="s">
         <v>537</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>538</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G62" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="10" t="s">
         <v>541</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="K62" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="K62" s="5" t="s">
+    </row>
+    <row r="63" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="12" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="129.6">
-      <c r="A63" s="12" t="s">
+      <c r="B63" s="12" t="s">
         <v>544</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="C63" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="18" t="s">
         <v>547</v>
-      </c>
-      <c r="E63" s="18" t="s">
-        <v>548</v>
       </c>
       <c r="F63" s="19">
         <v>10.8</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="J63" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="K63" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="K63" s="5" t="s">
+    </row>
+    <row r="64" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="12" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="259.14999999999998">
-      <c r="A64" s="12" t="s">
+      <c r="B64" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="B64" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="18" t="s">
         <v>556</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="F64" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="G64" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="J64" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="K64" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="K64" s="5" t="s">
+    </row>
+    <row r="65" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="115.15">
-      <c r="A65" s="12" t="s">
+      <c r="B65" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="B65" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="18" t="s">
         <v>566</v>
-      </c>
-      <c r="E65" s="18" t="s">
-        <v>567</v>
       </c>
       <c r="F65" s="19">
         <v>10.8</v>
       </c>
       <c r="G65" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="I65" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="K65" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="K65" s="5" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="172.9">
-      <c r="A66" s="12" t="s">
-        <v>572</v>
-      </c>
       <c r="B66" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>98</v>
@@ -6692,68 +6693,68 @@
         <v>98</v>
       </c>
       <c r="E66" s="18" t="s">
+        <v>572</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F66" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="K66" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="115.15">
-      <c r="A67" s="12" t="s">
+      <c r="B67" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="18" t="s">
+        <v>572</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="E67" s="18" t="s">
-        <v>573</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="G67" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="J67" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="K67" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="12" t="s">
         <v>583</v>
       </c>
-      <c r="K67" s="5" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="115.15">
-      <c r="A68" s="12" t="s">
-        <v>584</v>
-      </c>
       <c r="B68" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>98</v>
@@ -6762,655 +6763,655 @@
         <v>98</v>
       </c>
       <c r="E68" s="18" t="s">
+        <v>584</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="F68" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="G68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="I68" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="J68" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="5" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="K68" s="5" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="5" customFormat="1" ht="115.15">
-      <c r="A69" s="5" t="s">
-        <v>590</v>
-      </c>
       <c r="B69" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D69" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="F69" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="G69" s="5" t="s">
+      <c r="H69" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="J69" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="K69" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="5" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="K69" s="5" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" s="5" customFormat="1" ht="244.9">
-      <c r="A70" s="5" t="s">
+      <c r="B70" s="5" t="s">
         <v>597</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>598</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="6" t="s">
         <v>600</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="G70" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="H70" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="J70" s="9" t="s">
         <v>604</v>
       </c>
-      <c r="J70" s="9" t="s">
+      <c r="K70" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="K70" s="5" t="s">
+    </row>
+    <row r="71" spans="1:11" s="5" customFormat="1" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" s="5" customFormat="1" ht="316.89999999999998">
-      <c r="A71" s="5" t="s">
+      <c r="B71" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="G71" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="H71" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="J71" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="J71" s="9" t="s">
+      <c r="K71" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="K71" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="5" customFormat="1" ht="187.15">
-      <c r="A72" s="5" t="s">
+      <c r="B72" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="G72" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="H72" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="K72" s="5" t="s">
         <v>624</v>
       </c>
-      <c r="K72" s="5" t="s">
+    </row>
+    <row r="73" spans="1:11" s="5" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" s="5" customFormat="1" ht="158.44999999999999">
-      <c r="A73" s="5" t="s">
+      <c r="B73" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="F73" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="G73" s="5" t="s">
+      <c r="H73" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="J73" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="K73" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="K73" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" s="5" customFormat="1" ht="72">
-      <c r="A74" s="5" t="s">
+      <c r="B74" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="G74" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="G74" s="5" t="s">
+      <c r="H74" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="K74" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="5" customFormat="1" ht="360" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="K74" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="5" customFormat="1" ht="360">
-      <c r="A75" s="5" t="s">
+      <c r="B75" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="E75" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="F75" s="5" t="s">
+      <c r="G75" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="G75" s="5" t="s">
+      <c r="H75" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="J75" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="K75" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="K75" s="5" t="s">
+    </row>
+    <row r="76" spans="1:11" s="5" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" s="5" customFormat="1" ht="172.9">
-      <c r="A76" s="5" t="s">
+      <c r="B76" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="F76" s="5" t="s">
+      <c r="G76" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="G76" s="5" t="s">
+      <c r="H76" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="J76" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="K76" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="K76" s="5" t="s">
+    </row>
+    <row r="77" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="11" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" ht="115.15">
-      <c r="A77" s="11" t="s">
+      <c r="B77" s="12" t="s">
         <v>657</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="C77" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>660</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>661</v>
       </c>
       <c r="F77" s="12">
         <v>12.4</v>
       </c>
       <c r="G77" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I77" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="H77" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I77" s="2" t="s">
+      <c r="J77" s="9" t="s">
         <v>663</v>
       </c>
-      <c r="J77" s="9" t="s">
+      <c r="K77" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="K77" s="5" t="s">
+    </row>
+    <row r="78" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="11" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="115.15">
-      <c r="A78" s="11" t="s">
+      <c r="B78" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="B78" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="9" t="s">
         <v>670</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="H78" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="H78" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I78" s="2" t="s">
+      <c r="J78" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="K78" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="11" t="s">
         <v>673</v>
       </c>
-      <c r="K78" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="172.9">
-      <c r="A79" s="11" t="s">
+      <c r="B79" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="B79" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="H79" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I79" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="H79" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="K79" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="K79" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="409.6">
-      <c r="A80" s="11" t="s">
+      <c r="B80" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="B80" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="G80" s="9" t="s">
         <v>686</v>
       </c>
-      <c r="G80" s="9" t="s">
+      <c r="H80" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I80" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="H80" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I80" s="2" t="s">
+      <c r="J80" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="J80" s="3" t="s">
+      <c r="K80" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="288" x14ac:dyDescent="0.3">
+      <c r="A81" s="11" t="s">
         <v>689</v>
       </c>
-      <c r="K80" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="288">
-      <c r="A81" s="11" t="s">
+      <c r="B81" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="B81" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="G81" s="9" t="s">
+      <c r="H81" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I81" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="H81" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I81" s="2" t="s">
+      <c r="J81" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="K81" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="11" t="s">
         <v>696</v>
       </c>
-      <c r="K81" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="259.14999999999998">
-      <c r="A82" s="11" t="s">
+      <c r="B82" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="B82" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="9" t="s">
         <v>701</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="H82" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I82" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="H82" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I82" s="4" t="s">
+      <c r="J82" s="3" t="s">
         <v>703</v>
       </c>
-      <c r="J82" s="3" t="s">
+      <c r="K82" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="288" x14ac:dyDescent="0.3">
+      <c r="A83" s="11" t="s">
         <v>704</v>
       </c>
-      <c r="K82" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="288">
-      <c r="A83" s="11" t="s">
+      <c r="B83" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="B83" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="F83" s="9" t="s">
+      <c r="G83" s="9" t="s">
         <v>709</v>
       </c>
-      <c r="G83" s="9" t="s">
+      <c r="H83" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I83" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="H83" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I83" s="2" t="s">
+      <c r="J83" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="K83" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
         <v>712</v>
       </c>
-      <c r="K83" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="187.15">
-      <c r="A84" s="11" t="s">
+      <c r="B84" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="B84" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="D84" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>714</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>715</v>
       </c>
       <c r="F84" s="12">
         <v>3.4</v>
       </c>
       <c r="G84" s="9" t="s">
+        <v>715</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="H84" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I84" s="2" t="s">
+      <c r="J84" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="K84" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="11" t="s">
         <v>718</v>
       </c>
-      <c r="K84" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="129.6">
-      <c r="A85" s="11" t="s">
+      <c r="B85" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="G85" s="9" t="s">
         <v>723</v>
       </c>
-      <c r="G85" s="9" t="s">
+      <c r="H85" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="H85" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I85" s="2" t="s">
+      <c r="J85" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="J85" s="9" t="s">
+      <c r="K85" s="5" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A86" s="11" t="s">
         <v>726</v>
       </c>
-      <c r="K85" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="302.45">
-      <c r="A86" s="11" t="s">
+      <c r="B86" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="G86" s="9" t="s">
         <v>731</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="H86" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I86" s="9" t="s">
         <v>732</v>
       </c>
-      <c r="H86" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I86" s="9" t="s">
+      <c r="J86" s="9" t="s">
         <v>733</v>
       </c>
-      <c r="J86" s="9" t="s">
-        <v>734</v>
-      </c>
       <c r="K86" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>